<commit_message>
add fixtures/data_file_2_same_as_1.xlsx, a copy of fixtures/data_file_1.xlsx
</commit_message>
<xml_diff>
--- a/tests/fixtures/data_file_1.xlsx
+++ b/tests/fixtures/data_file_1.xlsx
@@ -7,13 +7,15 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Git metadata" sheetId="1" r:id="rId1"/>
-    <sheet name="Tests" sheetId="2" r:id="rId2"/>
-    <sheet name="References" sheetId="3" r:id="rId3"/>
+    <sheet name="Table of contents" sheetId="1" r:id="rId1"/>
+    <sheet name="Git metadata" sheetId="2" r:id="rId2"/>
+    <sheet name="Tests" sheetId="3" r:id="rId3"/>
+    <sheet name="References" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">References!$A$1:$B$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tests!$A$1:$D$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">References!$A$1:$B$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Table of contents'!$A$1:$C$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Tests!$A$1:$D$2</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -178,7 +180,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+  <si>
+    <t>'Git metadata'!A1</t>
+  </si>
+  <si>
+    <t>'Tests'!A1</t>
+  </si>
+  <si>
+    <t>'References'!A1</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Number of objects</t>
+  </si>
+  <si>
+    <t>Git metadata</t>
+  </si>
+  <si>
+    <t>Tests</t>
+  </si>
+  <si>
+    <t>References</t>
+  </si>
   <si>
     <t>Url</t>
   </si>
@@ -205,9 +234,6 @@
   </si>
   <si>
     <t>Existing attr</t>
-  </si>
-  <si>
-    <t>References</t>
   </si>
   <si>
     <t>test_1</t>
@@ -590,9 +616,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.01" customHeight="1" zeroHeight="1"/>
+  <cols>
+    <col min="1" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="16384" width="0" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.01" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.01" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.01" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.01" customHeight="1">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
+  <autoFilter ref="A1:C4"/>
+  <hyperlinks>
+    <hyperlink ref="A2" location="'Git metadata'!A1" tooltip="Click to view git metadata" display="'Git metadata'!A1"/>
+    <hyperlink ref="A3" location="'Tests'!A1" tooltip="Click to view tests" display="'Tests'!A1"/>
+    <hyperlink ref="A4" location="'References'!A1" tooltip="Click to view references" display="'References'!A1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -605,26 +696,26 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.01" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.01" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.01" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -645,7 +736,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -662,30 +753,30 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.01" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.01" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -710,7 +801,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -727,15 +818,15 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.01" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.01" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B2" s="3" t="b">
         <v>1</v>
@@ -743,7 +834,7 @@
     </row>
     <row r="3" spans="1:2" ht="15.01" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B3" s="3" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
add Git repo metadata to these files
</commit_message>
<xml_diff>
--- a/tests/fixtures/data_file_1.xlsx
+++ b/tests/fixtures/data_file_1.xlsx
@@ -1,23 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28109"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur_at_sinai/gitOnMyLaptopLocal/wc_dev_repos/test_repo/tests/fixtures/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="1920" yWindow="9980" windowWidth="16100" windowHeight="9660" activeTab="1"/>
+    <workbookView xWindow="-21500" yWindow="10540" windowWidth="18040" windowHeight="9220" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Table of contents" sheetId="1" r:id="rId1"/>
-    <sheet name="Git metadata" sheetId="2" r:id="rId2"/>
-    <sheet name="Tests" sheetId="3" r:id="rId3"/>
-    <sheet name="References" sheetId="4" r:id="rId4"/>
+    <sheet name="Data repo metadata" sheetId="6" r:id="rId2"/>
+    <sheet name="Schema repo metadata" sheetId="5" r:id="rId3"/>
+    <sheet name="Tests" sheetId="3" r:id="rId4"/>
+    <sheet name="References" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">References!$A$1:$B$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Table of contents'!$A$1:$C$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Tests!$A$1:$D$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">References!$A$1:$B$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Table of contents'!$A$1:$C$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Tests!$A$1:$D$2</definedName>
   </definedNames>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" iterateDelta="1E-4" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -88,50 +103,36 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Enter a unique string identifier that (1) starts with a letter, (2) is composed of letters, numbers and underscores, and (3) is less than 64 characters long
-Enter a string.
-Value must be between 1 and 63 characters.
-Value must be unique.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
           <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Enter an integer.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Enter a comma-separated list of values from "References:A" or blank.</t>
+    <comment ref="A2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Enter a string.
+Value must be less than or equal to 255 characters.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Enter a string.
+Value must be less than or equal to 255 characters.</t>
         </r>
       </text>
     </comment>
@@ -170,6 +171,72 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Enter a string.
+Value must be less than or equal to 255 characters.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Enter an integer.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Enter a comma-separated list of values from "References:A" or blank.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Enter a unique string identifier that (1) starts with a letter, (2) is composed of letters, numbers and underscores, and (3) is less than 64 characters long
+Enter a string.
+Value must be between 1 and 63 characters.
+Value must be unique.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>Enter a Boolean value
 Select "True" or "False".</t>
         </r>
@@ -180,16 +247,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
-  <si>
-    <t>'Git metadata'!A1</t>
-  </si>
-  <si>
-    <t>'Tests'!A1</t>
-  </si>
-  <si>
-    <t>'References'!A1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>Table</t>
   </si>
@@ -200,9 +258,6 @@
     <t>Number of objects</t>
   </si>
   <si>
-    <t>Git metadata</t>
-  </si>
-  <si>
     <t>Tests</t>
   </si>
   <si>
@@ -253,12 +308,24 @@
   <si>
     <t>ref_2</t>
   </si>
+  <si>
+    <t>Schema repo metadata</t>
+  </si>
+  <si>
+    <t>Data repo metadata</t>
+  </si>
+  <si>
+    <t>https://github.com/KarrLab/test_repo.git</t>
+  </si>
+  <si>
+    <t>a95d2f04b341e2c88bd92e03b121e4268119cf56</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,13 +341,13 @@
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -312,9 +379,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -328,6 +394,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -374,12 +445,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -406,14 +477,15 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -440,6 +512,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -615,119 +688,131 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" sqref="A1:A1048576"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.01" customHeight="1" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="16384" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.01" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.01" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.01" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.01" customHeight="1">
-      <c r="A4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
-  <autoFilter ref="A1:C4"/>
+  <sheetProtection insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
+  <autoFilter ref="A1:C5"/>
   <hyperlinks>
-    <hyperlink ref="A2" location="'Git metadata'!A1" tooltip="Click to view git metadata" display="'Git metadata'!A1"/>
-    <hyperlink ref="A3" location="'Tests'!A1" tooltip="Click to view tests" display="'Tests'!A1"/>
-    <hyperlink ref="A4" location="'References'!A1" tooltip="Click to view references" display="'References'!A1"/>
+    <hyperlink ref="A4" location="'Tests'!A1" tooltip="Click to view tests" display="'Tests'!A1"/>
+    <hyperlink ref="A5" location="'References'!A1" tooltip="Click to view references" display="'References'!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <selection pane="topRight" activeCell="B2" sqref="B2"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.01" customHeight="1" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="16384" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.01" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.01" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.01" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>14</v>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
+  <sheetProtection insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
   <dataValidations count="3">
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Url" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Url" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B1">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Url" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Url" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B3">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Branch" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Branch" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B2">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Revision" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Revision" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B2">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Revision" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Revision" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B3">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Branch" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Branch" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B1">
       <formula1>255</formula1>
     </dataValidation>
   </dataValidations>
@@ -737,57 +822,119 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A3" sqref="A3"/>
+    </sheetView>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="1">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" customWidth="1"/>
+    <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
+  <dataValidations count="3">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Url" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Url" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B3">
+      <formula1>255</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Revision" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Revision" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B2">
+      <formula1>255</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Branch" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Branch" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B1">
+      <formula1>255</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.01" customHeight="1" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="16384" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.01" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.01" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="3">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
   <autoFilter ref="A1:D2"/>
   <dataValidations count="4">
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (1) starts with a letter, (2) is composed of letters, numbers and underscores, and (3) is less than 64 characters long&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a unique string identifier that (1) starts with a letter, (2) is composed of letters, numbers and underscores, and (3) is less than 64 characters long&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value must be unique." sqref="A2">
+    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (1) starts with a letter, (2) is composed of letters, numbers and underscores, and (3) is less than 64 characters long_x000a__x000a_Value must be a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value must be unique." promptTitle="Id" prompt="Enter a unique string identifier that (1) starts with a letter, (2) is composed of letters, numbers and underscores, and (3) is less than 64 characters long_x000a__x000a_Enter a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value must be unique." sqref="A2">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B2">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B2">
       <formula1>255</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Existing attr" error="Value must be an integer." promptTitle="Existing attr" prompt="Enter an integer." sqref="C2">
@@ -801,42 +948,43 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.01" customHeight="1" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="16384" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.01" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.01" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="3" t="b">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.01" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="3" t="b">
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2" t="b">
         <v>0</v>
       </c>
     </row>
@@ -844,11 +992,11 @@
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
   <autoFilter ref="A1:B3"/>
   <dataValidations count="2">
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (1) starts with a letter, (2) is composed of letters, numbers and underscores, and (3) is less than 64 characters long&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a unique string identifier that (1) starts with a letter, (2) is composed of letters, numbers and underscores, and (3) is less than 64 characters long&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value must be unique." sqref="A2:A3">
+    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (1) starts with a letter, (2) is composed of letters, numbers and underscores, and (3) is less than 64 characters long_x000a__x000a_Value must be a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value must be unique." promptTitle="Id" prompt="Enter a unique string identifier that (1) starts with a letter, (2) is composed of letters, numbers and underscores, and (3) is less than 64 characters long_x000a__x000a_Enter a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value must be unique." sqref="A2:A3">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Published" error="Enter a Boolean value&#10;&#10;Value must be &quot;True&quot; or &quot;False&quot;." promptTitle="Published" prompt="Enter a Boolean value&#10;&#10;Select &quot;True&quot; or &quot;False&quot;." sqref="B2:B3">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Published" error="Enter a Boolean value_x000a__x000a_Value must be &quot;True&quot; or &quot;False&quot;." promptTitle="Published" prompt="Enter a Boolean value_x000a__x000a_Select &quot;True&quot; or &quot;False&quot;." sqref="B2:B3">
       <formula1>"True,False"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>